<commit_message>
Full test trước khi báo cáo
</commit_message>
<xml_diff>
--- a/QDMarketPlace/wwwroot/uploaded/excels/ProductImport.xlsx
+++ b/QDMarketPlace/wwwroot/uploaded/excels/ProductImport.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\messi\OneDrive - 1DriveVN\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB4C5F8-5AAA-4D00-9FB1-9E697F27F66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C719410F-7740-47DA-A5B1-FE389A5F7DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2895" yWindow="2895" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterateDelta="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Description</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Home Flag</t>
   </si>
   <si>
-    <t xml:space="preserve">Dawn of War </t>
-  </si>
-  <si>
     <t>Vĩnh viễn</t>
   </si>
   <si>
@@ -70,6 +67,12 @@
   </si>
   <si>
     <t>Daw of War SEO</t>
+  </si>
+  <si>
+    <t>Dawn of War 1</t>
+  </si>
+  <si>
+    <t>Dawn of War 2</t>
   </si>
 </sst>
 </file>
@@ -407,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,10 +468,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
       </c>
       <c r="C2">
         <v>390000</v>
@@ -480,21 +483,56 @@
         <v>400000</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>
       </c>
       <c r="K2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>390000</v>
+      </c>
+      <c r="D3">
+        <v>420000</v>
+      </c>
+      <c r="E3">
+        <v>400000</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>